<commit_message>
Reworked script with improved concatenation mechanism
</commit_message>
<xml_diff>
--- a/CETAF_DEVELOPMENTS/elasticsearch/cetaf_website_elastic_search/MARS_ES_DATA_FLOW/parse_mars/mars_model_20210206_mapping.xlsx
+++ b/CETAF_DEVELOPMENTS/elasticsearch/cetaf_website_elastic_search/MARS_ES_DATA_FLOW/parse_mars/mars_model_20210206_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1_root_institution.txt" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="1067">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="1068">
   <si>
     <t>field</t>
   </si>
@@ -2871,9 +2871,6 @@
     <t>yes -cluster</t>
   </si>
   <si>
-    <t>institution_address</t>
-  </si>
-  <si>
     <t>institution_address/postcode</t>
   </si>
   <si>
@@ -2919,9 +2916,6 @@
     <t>duplicate in ES + use "dir_rep_category" to distinguish director or deputy</t>
   </si>
   <si>
-    <t>organisation</t>
-  </si>
-  <si>
     <t>organisation/direction_governing_and_executive_bodies</t>
   </si>
   <si>
@@ -2949,9 +2943,6 @@
     <t>use field name in data + concatenate</t>
   </si>
   <si>
-    <t>organisation/director_or_legal_representative</t>
-  </si>
-  <si>
     <t>organisation/director_or_legal_representative/dir_rep_title</t>
   </si>
   <si>
@@ -3232,6 +3223,18 @@
   </si>
   <si>
     <t>es_concatenate_index</t>
+  </si>
+  <si>
+    <t>others :</t>
+  </si>
+  <si>
+    <t>es_concatenation_character</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -3615,8 +3618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3648,19 +3651,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>984</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1064</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>987</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>929</v>
@@ -3677,7 +3680,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3691,35 +3694,35 @@
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3733,7 +3736,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3747,10 +3750,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F7" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G7" t="s">
         <v>931</v>
@@ -3767,10 +3770,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F8" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G8" t="s">
         <v>932</v>
@@ -3787,10 +3790,10 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F9" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G9" t="s">
         <v>926</v>
@@ -3807,10 +3810,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F10" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G10" t="s">
         <v>925</v>
@@ -3827,10 +3830,10 @@
         <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F11" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G11" t="s">
         <v>928</v>
@@ -3847,13 +3850,13 @@
         <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F12" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G12" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3867,7 +3870,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="K13" t="s">
         <v>933</v>
@@ -3884,7 +3887,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="K14" t="s">
         <v>934</v>
@@ -3901,7 +3904,7 @@
         <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3915,10 +3918,10 @@
         <v>31</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F16" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G16" t="s">
         <v>935</v>
@@ -3944,10 +3947,10 @@
         <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F17" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G17" t="s">
         <v>936</v>
@@ -3976,10 +3979,10 @@
         <v>35</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F18" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G18" t="s">
         <v>935</v>
@@ -4005,10 +4008,10 @@
         <v>37</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F19" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G19" t="s">
         <v>936</v>
@@ -4034,10 +4037,10 @@
         <v>39</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F20" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G20" t="s">
         <v>935</v>
@@ -4063,10 +4066,10 @@
         <v>41</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F21" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G21" t="s">
         <v>936</v>
@@ -4092,7 +4095,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -4106,7 +4109,7 @@
         <v>44</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="K23" t="s">
         <v>937</v>
@@ -4123,7 +4126,7 @@
         <v>47</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -4137,7 +4140,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="K25" t="s">
         <v>940</v>
@@ -4154,7 +4157,7 @@
         <v>50</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="K26" t="s">
         <v>939</v>
@@ -4174,10 +4177,10 @@
         <v>52</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="F27" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G27" t="s">
         <v>927</v>
@@ -7359,10 +7362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+    <sheetView tabSelected="1" topLeftCell="G37" workbookViewId="0">
+      <selection activeCell="L68" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7373,16 +7376,19 @@
     <col min="4" max="4" width="109.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="165.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="53.28515625" customWidth="1"/>
-    <col min="7" max="8" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.42578125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="4" customWidth="1"/>
     <col min="11" max="11" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" customWidth="1"/>
-    <col min="13" max="13" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="14" max="14" width="66.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7399,40 +7405,43 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>1062</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>1065</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>985</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>984</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>986</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>1064</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>1065</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>1066</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>989</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>987</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>988</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1041</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -7443,13 +7452,14 @@
         <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -7460,13 +7470,14 @@
         <v>54</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -7477,25 +7488,23 @@
         <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F4" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G4" t="s">
         <v>942</v>
-      </c>
-      <c r="H4" t="s">
-        <v>946</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-      <c r="M4" t="s">
+      <c r="L4" s="6"/>
+      <c r="N4" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -7506,25 +7515,23 @@
         <v>58</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F5" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G5" t="s">
         <v>943</v>
-      </c>
-      <c r="H5" t="s">
-        <v>946</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-      <c r="M5" t="s">
+      <c r="L5" s="6"/>
+      <c r="N5" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -7535,25 +7542,23 @@
         <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F6" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G6" t="s">
-        <v>949</v>
-      </c>
-      <c r="H6" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-      <c r="M6" t="s">
+      <c r="L6" s="6"/>
+      <c r="N6" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -7564,25 +7569,23 @@
         <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F7" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G7" t="s">
-        <v>950</v>
-      </c>
-      <c r="H7" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-      <c r="M7" t="s">
+      <c r="L7" s="6"/>
+      <c r="N7" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -7593,25 +7596,23 @@
         <v>64</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F8" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G8" t="s">
-        <v>947</v>
-      </c>
-      <c r="H8" t="s">
         <v>946</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="M8" t="s">
+      <c r="L8" s="6"/>
+      <c r="N8" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -7622,25 +7623,23 @@
         <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F9" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G9" t="s">
-        <v>948</v>
-      </c>
-      <c r="H9" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="M9" t="s">
+      <c r="L9" s="6"/>
+      <c r="N9" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -7651,13 +7650,14 @@
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -7668,30 +7668,37 @@
         <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F11" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G11" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H11" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I11" s="6">
         <v>1</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="M11" t="s">
-        <v>953</v>
+      <c r="J11" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="N11" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+      <c r="O11" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -7702,27 +7709,37 @@
         <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F12" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G12" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H12" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I12" s="6">
         <v>1</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="M12" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="N12" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -7733,24 +7750,25 @@
         <v>73</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F13" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G13" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H13" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I13" s="6">
         <v>1</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -7761,31 +7779,34 @@
         <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F14" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G14" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H14" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K14" s="6">
-        <v>1</v>
-      </c>
-      <c r="N14" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O14" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -7796,31 +7817,34 @@
         <v>77</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F15" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G15" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H15" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I15" s="6">
         <v>1</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K15" s="6">
-        <v>1</v>
-      </c>
-      <c r="N15" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O15" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -7831,13 +7855,14 @@
         <v>79</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -7848,24 +7873,25 @@
         <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F17" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G17" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H17" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I17" s="6">
         <v>1</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -7876,24 +7902,25 @@
         <v>83</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F18" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G18" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="H18" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I18" s="6">
         <v>1</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -7904,24 +7931,25 @@
         <v>85</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F19" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H19" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I19" s="6">
         <v>1</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -7929,24 +7957,25 @@
         <v>6</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F20" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G20" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="H20" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I20" s="6">
         <v>1</v>
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -7957,30 +7986,37 @@
         <v>87</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F21" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G21" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H21" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I21" s="6">
         <v>2</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="M21" t="s">
-        <v>953</v>
+      <c r="J21" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K21" s="6">
+        <v>2</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="N21" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+      <c r="O21" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -7991,27 +8027,37 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F22" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G22" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H22" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I22" s="6">
         <v>2</v>
       </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="M22" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K22" s="6">
+        <v>2</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>1066</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>1064</v>
+      </c>
+      <c r="N22" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -8022,24 +8068,25 @@
         <v>90</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F23" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G23" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H23" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I23" s="6">
         <v>2</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -8050,31 +8097,34 @@
         <v>92</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F24" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G24" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H24" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I24" s="6">
         <v>2</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K24" s="6">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O24" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -8085,31 +8135,34 @@
         <v>94</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F25" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G25" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H25" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="I25" s="6">
         <v>2</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K25" s="6">
-        <v>2</v>
-      </c>
-      <c r="N25" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>1067</v>
+      </c>
+      <c r="O25" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -8120,13 +8173,14 @@
         <v>14</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -8137,22 +8191,25 @@
         <v>14</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F27" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G27" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H27" t="s">
-        <v>951</v>
-      </c>
-      <c r="I27" s="6"/>
+        <v>950</v>
+      </c>
+      <c r="I27" s="6">
+        <v>2</v>
+      </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -8163,22 +8220,25 @@
         <v>98</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F28" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G28" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="H28" t="s">
-        <v>951</v>
-      </c>
-      <c r="I28" s="6"/>
+        <v>950</v>
+      </c>
+      <c r="I28" s="6">
+        <v>2</v>
+      </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -8189,13 +8249,14 @@
         <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -8206,19 +8267,20 @@
         <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F30" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G30" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -8229,22 +8291,20 @@
         <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F31" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G31" t="s">
-        <v>963</v>
-      </c>
-      <c r="H31" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -8255,22 +8315,20 @@
         <v>14</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F32" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G32" t="s">
-        <v>965</v>
-      </c>
-      <c r="H32" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L32" s="6"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -8281,22 +8339,20 @@
         <v>14</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F33" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G33" t="s">
-        <v>966</v>
-      </c>
-      <c r="H33" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -8307,16 +8363,17 @@
         <v>104</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
-      <c r="N34" t="s">
+      <c r="L34" s="6"/>
+      <c r="O34" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -8327,22 +8384,20 @@
         <v>106</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F35" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G35" t="s">
-        <v>967</v>
-      </c>
-      <c r="H35" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -8353,22 +8408,20 @@
         <v>108</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F36" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G36" t="s">
-        <v>968</v>
-      </c>
-      <c r="H36" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>109</v>
       </c>
@@ -8379,13 +8432,14 @@
         <v>14</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L37" s="6"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
@@ -8396,13 +8450,14 @@
         <v>110</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>111</v>
       </c>
@@ -8413,28 +8468,26 @@
         <v>14</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F39" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G39" t="s">
-        <v>969</v>
-      </c>
-      <c r="H39" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
-      <c r="M39" t="s">
-        <v>953</v>
-      </c>
+      <c r="L39" s="6"/>
       <c r="N39" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+      <c r="O39" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -8445,16 +8498,17 @@
         <v>14</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
-      <c r="P40" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L40" s="6"/>
+      <c r="Q40" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -8465,28 +8519,26 @@
         <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F41" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G41" t="s">
-        <v>963</v>
-      </c>
-      <c r="H41" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
-      <c r="M41" t="s">
-        <v>953</v>
-      </c>
+      <c r="L41" s="6"/>
       <c r="N41" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+      <c r="O41" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -8497,28 +8549,26 @@
         <v>115</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F42" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G42" t="s">
-        <v>963</v>
-      </c>
-      <c r="H42" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
-      <c r="M42" t="s">
-        <v>953</v>
-      </c>
+      <c r="L42" s="6"/>
       <c r="N42" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>952</v>
+      </c>
+      <c r="O42" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -8529,25 +8579,25 @@
         <v>87</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F43" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G43" t="s">
-        <v>978</v>
-      </c>
-      <c r="H43" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
+      <c r="J43" s="6" t="s">
+        <v>952</v>
+      </c>
       <c r="K43" s="6"/>
-      <c r="M43" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L43" s="6"/>
+      <c r="N43" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -8558,25 +8608,25 @@
         <v>14</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F44" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G44" t="s">
-        <v>978</v>
-      </c>
-      <c r="H44" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
       <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
+      <c r="J44" s="6" t="s">
+        <v>952</v>
+      </c>
       <c r="K44" s="6"/>
-      <c r="M44" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L44" s="6"/>
+      <c r="N44" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>118</v>
       </c>
@@ -8587,25 +8637,23 @@
         <v>90</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F45" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G45" t="s">
-        <v>977</v>
-      </c>
-      <c r="H45" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
-      <c r="M45" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L45" s="6"/>
+      <c r="N45" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -8616,28 +8664,28 @@
         <v>92</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F46" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G46" t="s">
+        <v>973</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="N46" t="s">
         <v>976</v>
       </c>
-      <c r="H46" t="s">
-        <v>972</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="M46" t="s">
-        <v>979</v>
-      </c>
-      <c r="N46" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>120</v>
       </c>
@@ -8648,28 +8696,28 @@
         <v>94</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F47" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G47" t="s">
+        <v>973</v>
+      </c>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6" t="s">
+        <v>952</v>
+      </c>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="N47" t="s">
         <v>976</v>
       </c>
-      <c r="H47" t="s">
-        <v>972</v>
-      </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="M47" t="s">
-        <v>979</v>
-      </c>
-      <c r="N47" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>121</v>
       </c>
@@ -8680,16 +8728,13 @@
         <v>14</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>1033</v>
-      </c>
-      <c r="H48" t="s">
-        <v>972</v>
+        <v>1030</v>
       </c>
       <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
       <c r="K48" s="6"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L48" s="6"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -8700,25 +8745,23 @@
         <v>14</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F49" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G49" t="s">
-        <v>975</v>
-      </c>
-      <c r="H49" t="s">
         <v>972</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-      <c r="M49" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L49" s="6"/>
+      <c r="N49" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>123</v>
       </c>
@@ -8729,25 +8772,23 @@
         <v>124</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F50" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G50" t="s">
-        <v>974</v>
-      </c>
-      <c r="H50" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
-      <c r="M50" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L50" s="6"/>
+      <c r="N50" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>125</v>
       </c>
@@ -8758,25 +8799,23 @@
         <v>98</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F51" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G51" t="s">
-        <v>973</v>
-      </c>
-      <c r="H51" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
-      <c r="M51" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L51" s="6"/>
+      <c r="N51" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -8787,13 +8826,14 @@
         <v>44</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>126</v>
       </c>
@@ -8804,40 +8844,38 @@
         <v>128</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F53" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G53" t="s">
-        <v>969</v>
-      </c>
-      <c r="H53" t="s">
-        <v>962</v>
-      </c>
-      <c r="I53" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I53" s="6"/>
       <c r="J53" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K53" s="6">
         <v>1</v>
       </c>
-      <c r="L53" t="s">
-        <v>1043</v>
+      <c r="L53" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M53" t="s">
-        <v>953</v>
+        <v>1040</v>
       </c>
       <c r="N53" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O53" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P53" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -8848,40 +8886,38 @@
         <v>130</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F54" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G54" t="s">
-        <v>969</v>
-      </c>
-      <c r="H54" t="s">
-        <v>962</v>
-      </c>
-      <c r="I54" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I54" s="6"/>
       <c r="J54" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K54" s="6">
         <v>1</v>
       </c>
-      <c r="L54" t="s">
-        <v>1044</v>
+      <c r="L54" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M54" t="s">
-        <v>953</v>
+        <v>1041</v>
       </c>
       <c r="N54" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O54" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P54" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>131</v>
       </c>
@@ -8892,40 +8928,38 @@
         <v>132</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F55" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G55" t="s">
-        <v>969</v>
-      </c>
-      <c r="H55" t="s">
-        <v>962</v>
-      </c>
-      <c r="I55" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I55" s="6"/>
       <c r="J55" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K55" s="6">
         <v>1</v>
       </c>
-      <c r="L55" t="s">
-        <v>1045</v>
+      <c r="L55" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M55" t="s">
-        <v>953</v>
+        <v>1042</v>
       </c>
       <c r="N55" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O55" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P55" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>133</v>
       </c>
@@ -8936,40 +8970,38 @@
         <v>134</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F56" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G56" t="s">
-        <v>969</v>
-      </c>
-      <c r="H56" t="s">
-        <v>962</v>
-      </c>
-      <c r="I56" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I56" s="6"/>
       <c r="J56" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K56" s="6">
         <v>1</v>
       </c>
-      <c r="L56" t="s">
-        <v>1046</v>
+      <c r="L56" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M56" t="s">
-        <v>953</v>
+        <v>1043</v>
       </c>
       <c r="N56" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O56" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P56" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>135</v>
       </c>
@@ -8980,40 +9012,38 @@
         <v>136</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F57" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G57" t="s">
-        <v>969</v>
-      </c>
-      <c r="H57" t="s">
-        <v>962</v>
-      </c>
-      <c r="I57" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I57" s="6"/>
       <c r="J57" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K57" s="6">
         <v>1</v>
       </c>
-      <c r="L57" t="s">
-        <v>1047</v>
+      <c r="L57" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M57" t="s">
-        <v>953</v>
+        <v>1044</v>
       </c>
       <c r="N57" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O57" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P57" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -9024,40 +9054,38 @@
         <v>138</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F58" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G58" t="s">
-        <v>969</v>
-      </c>
-      <c r="H58" t="s">
-        <v>962</v>
-      </c>
-      <c r="I58" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I58" s="6"/>
       <c r="J58" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K58" s="6">
         <v>1</v>
       </c>
-      <c r="L58" t="s">
-        <v>1048</v>
+      <c r="L58" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M58" t="s">
-        <v>953</v>
+        <v>1045</v>
       </c>
       <c r="N58" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O58" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P58" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>139</v>
       </c>
@@ -9068,40 +9096,38 @@
         <v>14</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F59" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G59" t="s">
-        <v>969</v>
-      </c>
-      <c r="H59" t="s">
-        <v>962</v>
-      </c>
-      <c r="I59" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I59" s="6"/>
       <c r="J59" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K59" s="6">
         <v>1</v>
       </c>
-      <c r="L59" t="s">
-        <v>1049</v>
+      <c r="L59" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M59" t="s">
-        <v>953</v>
+        <v>1046</v>
       </c>
       <c r="N59" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O59" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P59" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>140</v>
       </c>
@@ -9112,40 +9138,38 @@
         <v>14</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F60" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G60" t="s">
-        <v>969</v>
-      </c>
-      <c r="H60" t="s">
-        <v>962</v>
-      </c>
-      <c r="I60" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I60" s="6"/>
       <c r="J60" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K60" s="6">
         <v>1</v>
       </c>
-      <c r="L60" t="s">
-        <v>1050</v>
+      <c r="L60" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M60" t="s">
-        <v>953</v>
+        <v>1047</v>
       </c>
       <c r="N60" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O60" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P60" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -9156,40 +9180,38 @@
         <v>132</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F61" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G61" t="s">
-        <v>969</v>
-      </c>
-      <c r="H61" t="s">
-        <v>962</v>
-      </c>
-      <c r="I61" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I61" s="6"/>
       <c r="J61" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K61" s="6">
         <v>1</v>
       </c>
-      <c r="L61" t="s">
-        <v>1051</v>
+      <c r="L61" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M61" t="s">
-        <v>953</v>
+        <v>1048</v>
       </c>
       <c r="N61" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O61" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P61" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>142</v>
       </c>
@@ -9200,40 +9222,38 @@
         <v>143</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F62" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G62" t="s">
-        <v>969</v>
-      </c>
-      <c r="H62" t="s">
-        <v>962</v>
-      </c>
-      <c r="I62" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I62" s="6"/>
       <c r="J62" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K62" s="6">
         <v>1</v>
       </c>
-      <c r="L62" t="s">
-        <v>1052</v>
+      <c r="L62" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M62" t="s">
-        <v>953</v>
+        <v>1049</v>
       </c>
       <c r="N62" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O62" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P62" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>144</v>
       </c>
@@ -9244,40 +9264,38 @@
         <v>145</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F63" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G63" t="s">
-        <v>969</v>
-      </c>
-      <c r="H63" t="s">
-        <v>962</v>
-      </c>
-      <c r="I63" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I63" s="6"/>
       <c r="J63" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K63" s="6">
         <v>1</v>
       </c>
-      <c r="L63" t="s">
-        <v>1053</v>
+      <c r="L63" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M63" t="s">
-        <v>953</v>
+        <v>1050</v>
       </c>
       <c r="N63" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O63" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P63" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>146</v>
       </c>
@@ -9288,40 +9306,38 @@
         <v>147</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F64" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G64" t="s">
-        <v>969</v>
-      </c>
-      <c r="H64" t="s">
-        <v>962</v>
-      </c>
-      <c r="I64" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I64" s="6"/>
       <c r="J64" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K64" s="6">
         <v>1</v>
       </c>
-      <c r="L64" t="s">
-        <v>1054</v>
+      <c r="L64" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M64" t="s">
-        <v>953</v>
+        <v>1051</v>
       </c>
       <c r="N64" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O64" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P64" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -9332,40 +9348,38 @@
         <v>14</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F65" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G65" t="s">
-        <v>969</v>
-      </c>
-      <c r="H65" t="s">
-        <v>962</v>
-      </c>
-      <c r="I65" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I65" s="6"/>
       <c r="J65" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K65" s="6">
         <v>1</v>
       </c>
-      <c r="L65" t="s">
-        <v>1055</v>
+      <c r="L65" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M65" t="s">
-        <v>953</v>
+        <v>1052</v>
       </c>
       <c r="N65" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O65" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P65" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -9376,40 +9390,38 @@
         <v>14</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F66" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G66" t="s">
-        <v>969</v>
-      </c>
-      <c r="H66" t="s">
-        <v>962</v>
-      </c>
-      <c r="I66" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I66" s="6"/>
       <c r="J66" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K66" s="6">
         <v>1</v>
       </c>
-      <c r="L66" t="s">
-        <v>1056</v>
+      <c r="L66" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M66" t="s">
-        <v>953</v>
+        <v>1053</v>
       </c>
       <c r="N66" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O66" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P66" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>150</v>
       </c>
@@ -9420,40 +9432,38 @@
         <v>14</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F67" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G67" t="s">
-        <v>969</v>
-      </c>
-      <c r="H67" t="s">
-        <v>962</v>
-      </c>
-      <c r="I67" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I67" s="6"/>
       <c r="J67" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K67" s="6">
         <v>1</v>
       </c>
-      <c r="L67" t="s">
-        <v>1057</v>
+      <c r="L67" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M67" t="s">
-        <v>953</v>
+        <v>1054</v>
       </c>
       <c r="N67" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O67" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P67" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>151</v>
       </c>
@@ -9464,40 +9474,38 @@
         <v>14</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F68" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G68" t="s">
-        <v>969</v>
-      </c>
-      <c r="H68" t="s">
-        <v>962</v>
-      </c>
-      <c r="I68" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I68" s="6"/>
       <c r="J68" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K68" s="6">
         <v>1</v>
       </c>
-      <c r="L68" t="s">
-        <v>1058</v>
+      <c r="L68" s="6" t="s">
+        <v>1066</v>
       </c>
       <c r="M68" t="s">
-        <v>953</v>
+        <v>1055</v>
       </c>
       <c r="N68" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O68" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P68" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>152</v>
       </c>
@@ -9508,13 +9516,14 @@
         <v>14</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L69" s="6"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>153</v>
       </c>
@@ -9525,38 +9534,34 @@
         <v>154</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F70" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G70" t="s">
-        <v>969</v>
-      </c>
-      <c r="H70" t="s">
-        <v>962</v>
-      </c>
-      <c r="I70" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I70" s="6"/>
       <c r="J70" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K70" s="6"/>
-      <c r="L70" t="s">
-        <v>1059</v>
-      </c>
+      <c r="L70" s="6"/>
       <c r="M70" t="s">
-        <v>953</v>
+        <v>1056</v>
       </c>
       <c r="N70" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O70" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P70" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>155</v>
       </c>
@@ -9567,38 +9572,34 @@
         <v>156</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F71" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G71" t="s">
-        <v>969</v>
-      </c>
-      <c r="H71" t="s">
-        <v>962</v>
-      </c>
-      <c r="I71" s="6">
-        <v>1</v>
-      </c>
+        <v>967</v>
+      </c>
+      <c r="I71" s="6"/>
       <c r="J71" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="K71" s="6"/>
-      <c r="L71" t="s">
-        <v>1060</v>
-      </c>
+      <c r="L71" s="6"/>
       <c r="M71" t="s">
-        <v>953</v>
+        <v>1057</v>
       </c>
       <c r="N71" t="s">
-        <v>970</v>
+        <v>952</v>
       </c>
       <c r="O71" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+        <v>968</v>
+      </c>
+      <c r="P71" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>157</v>
       </c>
@@ -9609,22 +9610,20 @@
         <v>14</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F72" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G72" t="s">
-        <v>981</v>
-      </c>
-      <c r="H72" t="s">
-        <v>962</v>
+        <v>978</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>158</v>
       </c>
@@ -9635,39 +9634,38 @@
         <v>14</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F73" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G73" t="s">
-        <v>982</v>
-      </c>
-      <c r="H73" t="s">
-        <v>962</v>
+        <v>979</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L73" s="6"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L74" s="6"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -9678,22 +9676,20 @@
         <v>159</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F75" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G75" t="s">
-        <v>983</v>
-      </c>
-      <c r="H75" t="s">
-        <v>962</v>
+        <v>980</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L75" s="6"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>160</v>
       </c>
@@ -9704,22 +9700,20 @@
         <v>161</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="F76" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="G76" t="s">
-        <v>1063</v>
-      </c>
-      <c r="H76" t="s">
-        <v>962</v>
+        <v>1060</v>
       </c>
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L76" s="6"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>49</v>
       </c>
@@ -9730,7 +9724,7 @@
         <v>162</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
   </sheetData>
@@ -9786,7 +9780,7 @@
         <v>163</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -9800,7 +9794,7 @@
         <v>164</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -9814,7 +9808,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -9828,7 +9822,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -9842,7 +9836,7 @@
         <v>168</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -9856,7 +9850,7 @@
         <v>170</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -9870,7 +9864,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -9884,7 +9878,7 @@
         <v>173</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -9898,7 +9892,7 @@
         <v>175</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -9912,7 +9906,7 @@
         <v>177</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -9926,7 +9920,7 @@
         <v>179</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -9940,7 +9934,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -9954,7 +9948,7 @@
         <v>85</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -9968,7 +9962,7 @@
         <v>182</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -9979,7 +9973,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -9993,7 +9987,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -10007,7 +10001,7 @@
         <v>69</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -10021,7 +10015,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -10035,7 +10029,7 @@
         <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -10049,7 +10043,7 @@
         <v>187</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -10063,7 +10057,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -10077,7 +10071,7 @@
         <v>14</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -10091,7 +10085,7 @@
         <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -10105,7 +10099,7 @@
         <v>14</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -10119,7 +10113,7 @@
         <v>193</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -10133,7 +10127,7 @@
         <v>194</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -10147,7 +10141,7 @@
         <v>14</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -10161,7 +10155,7 @@
         <v>197</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -10175,7 +10169,7 @@
         <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -10189,7 +10183,7 @@
         <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -10203,7 +10197,7 @@
         <v>14</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -10217,7 +10211,7 @@
         <v>202</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -10231,7 +10225,7 @@
         <v>14</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -10245,7 +10239,7 @@
         <v>14</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -10259,7 +10253,7 @@
         <v>44</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -10273,7 +10267,7 @@
         <v>14</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -10287,7 +10281,7 @@
         <v>206</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -10301,7 +10295,7 @@
         <v>208</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -10315,7 +10309,7 @@
         <v>209</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -10329,7 +10323,7 @@
         <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -10343,7 +10337,7 @@
         <v>14</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -10357,7 +10351,7 @@
         <v>213</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>